<commit_message>
before implementing background removal
</commit_message>
<xml_diff>
--- a/scripts/test/bright_neighbor_results.xlsx
+++ b/scripts/test/bright_neighbor_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,133 +482,133 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5426587107145955712</t>
+          <t>4529285391522200320</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>142.6736805260494</v>
+        <v>275.9254491025025</v>
       </c>
       <c r="C2" t="n">
-        <v>-40.46642826305888</v>
+        <v>21.76870525491716</v>
       </c>
       <c r="D2" t="n">
-        <v>3.674772262573242</v>
+        <v>3.389339208602905</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>4529285391531266304</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>4.803853511810303</v>
+        <v>3.39525294303894</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0002820617191807018</v>
+        <v>0.0001677126147536809</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2756363608023335808</t>
+          <t>5426587107145955712</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>354.9892981679823</v>
+        <v>142.6736805260494</v>
       </c>
       <c r="C3" t="n">
-        <v>5.624412199677955</v>
+        <v>-40.46642826305888</v>
       </c>
       <c r="D3" t="n">
-        <v>3.924485921859741</v>
+        <v>3.674772262573242</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2756363608022656384</t>
+          <t>5426587107149861120</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>7.892950057983398</v>
+        <v>4.803853511810303</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001394960122499403</v>
+        <v>0.0002820617191807018</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1244571953471006720</t>
+          <t>4432032213656433536</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>206.8134593324645</v>
+        <v>247.7282713167697</v>
       </c>
       <c r="C4" t="n">
-        <v>17.45716469916912</v>
+        <v>1.983620889639908</v>
       </c>
       <c r="D4" t="n">
-        <v>4.294786930084229</v>
+        <v>4.066857814788818</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>1244571953470337280</t>
+          <t>4432032213656434176</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>9.46910572052002</v>
+        <v>6.452131748199463</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0004435041882477545</v>
+        <v>0.0003843007249245102</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6719152945029845376</t>
+          <t>6541802406664428672</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>286.6054157588619</v>
+        <v>346.7194246886781</v>
       </c>
       <c r="C5" t="n">
-        <v>-37.06488085942344</v>
+        <v>-43.52041179748344</v>
       </c>
       <c r="D5" t="n">
-        <v>4.717123985290527</v>
+        <v>4.234705448150635</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>6719152945032456832</t>
+          <t>6541802402371581568</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>4.760257244110107</v>
+        <v>6.503548145294189</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0003869906325269605</v>
+        <v>0.0004380720153890083</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>6719152945029845376</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>286.6054157588619</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-37.06488085942344</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4.717123985290527</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>6719152945032456832</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>286.6053079615535</v>
-      </c>
-      <c r="C6" t="n">
-        <v>-37.06450354954132</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="F6" t="n">
         <v>4.760257244110107</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>6719152945029845376</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>4.717123985290527</v>
       </c>
       <c r="G6" t="n">
         <v>0.0003869906325269605</v>
@@ -617,136 +617,325 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>5426587107149861120</t>
+          <t>6719152945032456832</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>142.6740032632142</v>
+        <v>286.6053079615535</v>
       </c>
       <c r="C7" t="n">
-        <v>-40.466567086598</v>
+        <v>-37.06450354954132</v>
       </c>
       <c r="D7" t="n">
-        <v>4.803853511810303</v>
+        <v>4.760257244110107</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>5426587107145955712</t>
+          <t>6719152945029845376</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>3.674772262573242</v>
+        <v>4.717123985290527</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0002820617191807018</v>
+        <v>0.0003869906325269605</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>6508776375901968640</t>
+          <t>4343066192373234048</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>334.5682592612844</v>
+        <v>241.0920131228604</v>
       </c>
       <c r="C8" t="n">
-        <v>-53.62978547970057</v>
+        <v>-11.37304460452119</v>
       </c>
       <c r="D8" t="n">
-        <v>5.210835456848145</v>
+        <v>4.767579555511475</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>6508776375900830592</t>
+          <t>4343066192367555200</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>9.186453819274902</v>
+        <v>4.771558284759521</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0005185029289548906</v>
+        <v>0.0003030379884824618</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4373199678620639744</t>
+          <t>4343066192367555200</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>262.5984522008857</v>
+        <v>241.0919870016956</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.063482522283796</v>
+        <v>-11.37334655855848</v>
       </c>
       <c r="D9" t="n">
-        <v>5.779087543487549</v>
+        <v>4.771558284759521</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>4373199682919087616</t>
+          <t>4343066192373234048</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>5.801146030426025</v>
+        <v>4.767579555511475</v>
       </c>
       <c r="G9" t="n">
-        <v>0.000199786113763143</v>
+        <v>0.0003030379884824618</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4373199682919087616</t>
+          <t>6860945174279114880</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>262.5985706282946</v>
+        <v>307.2149851888128</v>
       </c>
       <c r="C10" t="n">
-        <v>-1.063643439256715</v>
+        <v>-17.81372857084146</v>
       </c>
       <c r="D10" t="n">
-        <v>5.801146030426025</v>
+        <v>4.794205188751221</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>4373199678620639744</t>
+          <t>6860945174275852416</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>5.779087543487549</v>
+        <v>6.696762561798096</v>
       </c>
       <c r="G10" t="n">
-        <v>0.000199786113763143</v>
+        <v>0.0004518621805492849</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3213958769587525888</t>
+          <t>5426587107149861120</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>79.80577003837008</v>
+        <v>142.6740032632142</v>
       </c>
       <c r="C11" t="n">
-        <v>-3.073222913358394</v>
+        <v>-40.466567086598</v>
       </c>
       <c r="D11" t="n">
-        <v>7.478399753570557</v>
+        <v>4.803853511810303</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3213958769589070848</t>
+          <t>5426587107145955712</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>9.889883041381836</v>
+        <v>3.674772262573242</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0004238375517909563</v>
+        <v>0.0002820617191807018</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>657244586015485440</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>123.0535363160312</v>
+      </c>
+      <c r="C12" t="n">
+        <v>17.64700231993405</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5.410910606384277</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>657244521593509376</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>5.792698383331299</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.0003145394475308107</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>6724105656508792576</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>271.7079518856002</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-43.42567811693711</v>
+      </c>
+      <c r="D13" t="n">
+        <v>5.581056118011475</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>6724105660828668032</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>5.644303798675537</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.0004930990478208497</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>6724105660828668032</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>271.7079719599973</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-43.42518523347083</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5.644303798675537</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>6724105656508792576</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>5.581056118011475</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0004930990478208497</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2803936143261926272</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>13.74271321842037</v>
+      </c>
+      <c r="C15" t="n">
+        <v>23.62814488153855</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5.725862503051758</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2803936138967498624</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>6.123550891876221</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.0003119170200913206</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>4373199678620639744</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>262.5984522008857</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-1.063482522283796</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5.779087543487549</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>4373199682919087616</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>5.801146030426025</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.000199786113763143</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>657244521593509376</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>123.0536499059178</v>
+      </c>
+      <c r="C17" t="n">
+        <v>17.64729764719009</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5.792698383331299</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>657244586015485440</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>5.410910606384277</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0003145394475308107</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>4373199682919087616</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>262.5985706282946</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1.063643439256715</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5.801146030426025</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4373199678620639744</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>5.779087543487549</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.000199786113763143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>